<commit_message>
CM FEITO MY DUDES
deem scale depois though
</commit_message>
<xml_diff>
--- a/CM.xlsx
+++ b/CM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jose Murteira\Documents\ProjetoIntegrador\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D744286F-6FD4-4F47-BF5C-F824CD1CA52D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F63129C7-2660-4164-B1CC-50D4EC20AC7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BD71ADCE-B825-4B1A-BFDF-75C3D05E800C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="31">
   <si>
     <t>Objeto</t>
   </si>
@@ -104,6 +104,30 @@
   </si>
   <si>
     <t>Asa2</t>
+  </si>
+  <si>
+    <t>CM</t>
+  </si>
+  <si>
+    <t>Massa total</t>
+  </si>
+  <si>
+    <t>Motores 1</t>
+  </si>
+  <si>
+    <t>Combustivel 1</t>
+  </si>
+  <si>
+    <t>Combustivel 2</t>
+  </si>
+  <si>
+    <t>Baterias</t>
+  </si>
+  <si>
+    <t>Equipamento Médico</t>
+  </si>
+  <si>
+    <t>Aviónica</t>
   </si>
 </sst>
 </file>
@@ -119,7 +143,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -138,8 +162,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -188,19 +224,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -213,6 +272,37 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -235,16 +325,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>219520</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>857013</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>127747</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>173735</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>125009</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>367553</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>159517</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -267,8 +357,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9607360" y="2415540"/>
-          <a:ext cx="3611815" cy="1709969"/>
+          <a:off x="8163248" y="3883959"/>
+          <a:ext cx="5857552" cy="2721182"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -577,10 +667,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F1E2D37-831C-469B-8823-F05FC713D19C}">
-  <dimension ref="B2:O19"/>
+  <dimension ref="B2:S23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -595,7 +685,7 @@
     <col min="9" max="9" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:19" x14ac:dyDescent="0.3">
       <c r="D2" t="s">
         <v>19</v>
       </c>
@@ -606,169 +696,231 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="2:15" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:19" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3" t="s">
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="7" t="s">
+      <c r="G4" s="7"/>
+      <c r="H4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="8"/>
-      <c r="J4" s="3" t="s">
+      <c r="I4" s="6"/>
+      <c r="J4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="3"/>
-      <c r="L4" s="7" t="s">
+      <c r="K4" s="7"/>
+      <c r="L4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M4" s="8"/>
-      <c r="N4" s="3" t="s">
+      <c r="M4" s="6"/>
+      <c r="N4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="3"/>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B5" s="4" t="s">
+      <c r="O4" s="7"/>
+      <c r="P4" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q4" s="17"/>
+      <c r="R4" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="S4" s="17"/>
+    </row>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B5" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="C5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="N5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="O5" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B6" s="4"/>
-      <c r="C6" s="6">
-        <f>12970.19*(10^-3)+((958.07+929.88/2)*(3234.12-1035.11)*883.55+958.07*2420.38/2*958.07*2/3+1035.11*883.55/2*(958.07+883.55/3))*(10^-3)/(C8*(10^9)/200)</f>
+      <c r="F5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B6" s="8"/>
+      <c r="C6" s="4">
+        <f>12970.19*(10^-3)+((958.07+929.88/2)*(3234.12-1035.11)*883.55+958.07*2420.38/2*958.07*2/3+1035.11*883.55/2*(958.07+883.55/3))*(10^-3)/(C8*(10^9)/5)</f>
         <v>14.134862515166017</v>
       </c>
-      <c r="D6" s="6">
-        <f>2463.01*10^-3+((3234.12-1035.11)*883.55*(3234.12-1035.11)/2+958.07*2420.38/2*2420.38/3+1035.11*883.55/2*(-1035.11/3))*(10^-3)/(C8*(10^9)/200)</f>
+      <c r="D6" s="4">
+        <f>2463.01*10^-3+((3234.12-1035.11)*883.55*(3234.12-1035.11)/2+958.07*2420.38/2*2420.38/3+1035.11*883.55/2*(-1035.11/3))*(10^-3)/(C8*(10^9)/5)</f>
         <v>3.295189928858151</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="4">
         <v>0</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="4">
         <f>10465.49*10^-3+1065.08*10^-3</f>
         <v>11.530570000000001</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="4">
         <f>1491*10^-3</f>
         <v>1.4910000000000001</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="4">
         <f>(6943+676.98)*10^-3</f>
         <v>7.61998</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="4">
         <f>1009.86*10^-3</f>
         <v>1.00986</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="4">
         <f>(3033.52+7436.06/2)*10^-3</f>
         <v>6.7515499999999999</v>
       </c>
-      <c r="K6" s="6">
+      <c r="K6" s="4">
         <f>(2078.5/2*10^-3)</f>
         <v>1.03925</v>
       </c>
-      <c r="L6" s="6">
+      <c r="L6" s="4">
         <f>(1199.05+1383.26)*10^-3</f>
         <v>2.5823100000000001</v>
       </c>
-      <c r="M6" s="6">
+      <c r="M6" s="4">
         <f>742.05*10^-3</f>
         <v>0.74204999999999999</v>
       </c>
-      <c r="N6" s="6">
-        <v>921.78</v>
-      </c>
-      <c r="O6" s="6">
+      <c r="N6" s="4">
+        <f>921.78*10^-3</f>
+        <v>0.92178000000000004</v>
+      </c>
+      <c r="O6" s="4">
         <f>383.04*10^-3</f>
         <v>0.38304000000000005</v>
       </c>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="P6" s="4">
+        <v>6.28</v>
+      </c>
+      <c r="Q6" s="4">
+        <f>383.04*10^-3</f>
+        <v>0.38304000000000005</v>
+      </c>
+      <c r="R6" s="4">
+        <f>(1199.05+1383.26)/2*10^-3</f>
+        <v>1.2911550000000001</v>
+      </c>
+      <c r="S6" s="4">
+        <f>742.05*10^-3</f>
+        <v>0.74204999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="1"/>
+      <c r="C7" s="1">
+        <f>C9*C8</f>
+        <v>140.06204736200004</v>
+      </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="F7" s="1">
+        <f>F9*F8</f>
+        <v>387.91125840000001</v>
+      </c>
       <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
+      <c r="H7" s="1">
+        <f>H9*H8</f>
+        <v>213.03365896</v>
+      </c>
       <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
+      <c r="J7" s="1">
+        <f>J9*J8</f>
+        <v>268.59048720000004</v>
+      </c>
       <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
+      <c r="L7" s="1">
+        <f>L9*L8</f>
+        <v>303.80480120000004</v>
+      </c>
       <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
+      <c r="N7" s="1">
+        <f>N9*N8</f>
+        <v>87.45227392000001</v>
+      </c>
       <c r="O7" s="1"/>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="P7" s="1">
+        <v>185.59</v>
+      </c>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1">
+        <v>5</v>
+      </c>
+      <c r="S7" s="1"/>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="1">
-        <f>(((3234.12-1035.11)*883.55+1035.11*883.55/2+(929.88-883.55+955.33)/2*(3234.12-1035.11))*200)*10^-9</f>
-        <v>0.70031023681000015</v>
+        <f>(((3234.12-1035.11)*883.55+1035.11*883.55/2+(929.88-883.55+955.33)/2*(3234.12-1035.11))*5)*10^-9</f>
+        <v>1.7507755920250005E-2</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1">
-        <f>5624165687.92*10^-9</f>
-        <v>5.6241656879200006</v>
+        <f xml:space="preserve"> 48488907.3*10^-9</f>
+        <v>4.8488907300000002E-2</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1">
-        <f>5050279102.89*10^-9</f>
-        <v>5.0502791028900003</v>
+        <f xml:space="preserve"> 26629207.37 *10^-9</f>
+        <v>2.6629207370000001E-2</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1">
@@ -782,30 +934,55 @@
       </c>
       <c r="M8" s="1"/>
       <c r="N8" s="1">
-        <f>992872660.14*10^-9</f>
-        <v>0.99287266014000009</v>
+        <f>10931534.24 *10^-9</f>
+        <v>1.093153424E-2</v>
       </c>
       <c r="O8" s="1"/>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="1"/>
+      <c r="C9" s="1">
+        <v>8000</v>
+      </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+      <c r="F9" s="1">
+        <f>C9</f>
+        <v>8000</v>
+      </c>
       <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
+      <c r="H9" s="1">
+        <f>$C$9</f>
+        <v>8000</v>
+      </c>
       <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
+      <c r="J9" s="1">
+        <f>$C$9</f>
+        <v>8000</v>
+      </c>
       <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
+      <c r="L9" s="1">
+        <f>$C$9</f>
+        <v>8000</v>
+      </c>
       <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
+      <c r="N9" s="1">
+        <f>$C$9</f>
+        <v>8000</v>
+      </c>
       <c r="O9" s="1"/>
-    </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
@@ -828,56 +1005,207 @@
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="1" t="s">
+      <c r="D13" s="7"/>
+      <c r="E13" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1" t="s">
+      <c r="F13" s="11"/>
+      <c r="G13" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B14" s="4" t="s">
+      <c r="H13" s="11"/>
+      <c r="I13" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="L13" s="9"/>
+      <c r="M13" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="N13" s="11"/>
+      <c r="O13" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="R13" s="9"/>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B14" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B15" s="4"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="C14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="P14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R14" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B15" s="8"/>
+      <c r="C15" s="3">
+        <v>7.03</v>
+      </c>
+      <c r="D15" s="3">
+        <v>2.38</v>
+      </c>
+      <c r="E15" s="3">
+        <f>3.04+0.84</f>
+        <v>3.88</v>
+      </c>
+      <c r="F15" s="3">
+        <f>2.01+0.9</f>
+        <v>2.9099999999999997</v>
+      </c>
+      <c r="G15" s="3">
+        <f>0.84+12.09</f>
+        <v>12.93</v>
+      </c>
+      <c r="H15" s="3">
+        <f>2.53+0.9</f>
+        <v>3.4299999999999997</v>
+      </c>
+      <c r="I15" s="3">
+        <f>3.04+0.84-0.62</f>
+        <v>3.26</v>
+      </c>
+      <c r="J15" s="3">
+        <f>2.01+0.9</f>
+        <v>2.9099999999999997</v>
+      </c>
+      <c r="K15" s="3">
+        <f>0.84+12.09-0.62</f>
+        <v>12.31</v>
+      </c>
+      <c r="L15" s="3">
+        <f>2.53+0.9</f>
+        <v>3.4299999999999997</v>
+      </c>
+      <c r="M15" s="3">
+        <f>3.04+0.84</f>
+        <v>3.88</v>
+      </c>
+      <c r="N15" s="3">
+        <f>2.01+0.9</f>
+        <v>2.9099999999999997</v>
+      </c>
+      <c r="O15" s="3">
+        <f>0.84+12.09</f>
+        <v>12.93</v>
+      </c>
+      <c r="P15" s="3">
+        <f>2.53+0.9</f>
+        <v>3.4299999999999997</v>
+      </c>
+      <c r="Q15" s="4">
+        <v>6.28</v>
+      </c>
+      <c r="R15" s="4">
+        <f>1.5</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="1"/>
+      <c r="C16" s="1">
+        <v>200</v>
+      </c>
       <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
+      <c r="E16" s="1">
+        <v>200</v>
+      </c>
       <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
+      <c r="G16" s="1">
+        <v>200</v>
+      </c>
       <c r="H16" s="1"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I16" s="1">
+        <f>50*4</f>
+        <v>200</v>
+      </c>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1">
+        <f>50*4</f>
+        <v>200</v>
+      </c>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1">
+        <f>350</f>
+        <v>350</v>
+      </c>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1">
+        <f>350</f>
+        <v>350</v>
+      </c>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1">
+        <v>150</v>
+      </c>
+      <c r="R16" s="1"/>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
         <v>3</v>
       </c>
@@ -887,8 +1215,18 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
         <v>4</v>
       </c>
@@ -898,8 +1236,18 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
         <v>12</v>
       </c>
@@ -909,9 +1257,59 @@
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="C21" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="14"/>
+      <c r="F21" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="G21" s="14"/>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="C22" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="15">
+        <f>(C7+F7+H7+J7+L7+N7+C16+E16+G16+I16+K16+M16+O16+P7+Q16+R7)</f>
+        <v>3441.4445270420001</v>
+      </c>
+      <c r="G22" s="15"/>
+    </row>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="C23" s="12">
+        <f>(C6*C7+F6*F7+H6*H7+J6*J7+L6*L7+N6*N7+C15*C16+E15*E16+G15*G16+I15*I16+K15*K16+M15*M16+O15*O16+P6*P7+Q15*Q16+R6*R7)/F22</f>
+        <v>7.7391632278943643</v>
+      </c>
+      <c r="D23" s="12">
+        <f>(D6*C7+G6*F7+I6*H7+K6*J7+M6*L7+O6*D15*F15*H15*G16+J15*I16+L15*K16+N15*M16+P15*O16+Q6*P7+R15*Q16+S6*R7)/F22</f>
+        <v>2.1404591565015867</v>
+      </c>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="21">
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G23"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="K13:L13"/>
     <mergeCell ref="L4:M4"/>
     <mergeCell ref="N4:O4"/>
     <mergeCell ref="B14:B15"/>
@@ -921,6 +1319,13 @@
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="J4:K4"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="R4:S4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>